<commit_message>
New results from the code
</commit_message>
<xml_diff>
--- a/data/interim/Recipe_template.xlsx
+++ b/data/interim/Recipe_template.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paula\Downloads\Python basics\Project_V3\Python stuff\Thesis2024\data\interim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9080055-D25D-4F46-8091-E57F9AC0A1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CD310652-F69D-4C37-9A86-FC2CE3D80250}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -635,17 +634,17 @@
     <t>tbsp</t>
   </si>
   <si>
-    <t>cloves</t>
-  </si>
-  <si>
     <t>bunch</t>
+  </si>
+  <si>
+    <t>clove</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1018,19 +1017,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2F7C9C-161E-485E-BC60-5AA8CA50977D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1041,7 +1040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1049,7 +1048,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1057,7 +1056,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1065,7 +1064,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1073,7 +1072,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1081,7 +1080,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1089,7 +1088,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1097,7 +1096,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1105,7 +1104,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1113,7 +1112,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1121,7 +1120,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1129,7 +1128,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1137,7 +1136,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1145,7 +1144,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1153,7 +1152,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1161,7 +1160,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1169,7 +1168,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1177,7 +1176,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1185,7 +1184,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1193,7 +1192,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1204,7 +1203,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1212,7 +1211,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1223,7 +1222,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1231,7 +1230,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1239,7 +1238,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1247,7 +1246,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1255,7 +1254,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1271,7 +1270,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1279,7 +1278,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1287,7 +1286,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1295,7 +1294,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1303,7 +1302,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1311,7 +1310,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1319,7 +1318,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1327,7 +1326,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1335,7 +1334,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1343,7 +1342,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1351,7 +1350,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1359,7 +1358,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1367,7 +1366,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -1375,7 +1374,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1383,7 +1382,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -1391,7 +1390,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -1399,7 +1398,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1407,7 +1406,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1415,7 +1414,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1423,7 +1422,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1431,7 +1430,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1439,7 +1438,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1447,7 +1446,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1455,7 +1454,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1463,7 +1462,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1471,7 +1470,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1479,7 +1478,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1487,7 +1486,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1495,7 +1494,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1503,7 +1502,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1511,7 +1510,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1519,7 +1518,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1527,7 +1526,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1538,7 +1537,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1546,7 +1545,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -1554,7 +1553,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -1565,7 +1564,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -1573,7 +1572,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -1581,7 +1580,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -1589,7 +1588,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -1597,7 +1596,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -1608,7 +1607,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -1616,15 +1615,15 @@
         <v>197</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
       <c r="C72" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -1632,10 +1631,10 @@
         <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -1643,7 +1642,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -1651,7 +1650,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -1659,7 +1658,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -1667,7 +1666,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -1675,7 +1674,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -1683,7 +1682,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -1691,7 +1690,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -1699,7 +1698,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -1707,7 +1706,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -1715,7 +1714,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -1723,7 +1722,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -1731,7 +1730,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -1739,7 +1738,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -1747,7 +1746,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -1755,7 +1754,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -1763,7 +1762,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -1771,7 +1770,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -1779,7 +1778,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3">
       <c r="A92" t="s">
         <v>38</v>
       </c>
@@ -1787,7 +1786,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -1795,7 +1794,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -1803,7 +1802,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -1811,7 +1810,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -1819,7 +1818,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -1827,7 +1826,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
         <v>39</v>
       </c>
@@ -1835,7 +1834,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
         <v>96</v>
       </c>
@@ -1843,7 +1842,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
         <v>38</v>
       </c>
@@ -1851,7 +1850,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
         <v>97</v>
       </c>
@@ -1859,7 +1858,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
         <v>98</v>
       </c>
@@ -1867,7 +1866,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
         <v>99</v>
       </c>
@@ -1875,7 +1874,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>100</v>
       </c>
@@ -1883,7 +1882,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
         <v>101</v>
       </c>
@@ -1891,7 +1890,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
         <v>102</v>
       </c>
@@ -1899,7 +1898,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
         <v>103</v>
       </c>
@@ -1907,7 +1906,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
         <v>104</v>
       </c>
@@ -1915,7 +1914,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3">
       <c r="A109" t="s">
         <v>105</v>
       </c>
@@ -1923,7 +1922,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
         <v>106</v>
       </c>
@@ -1931,7 +1930,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3">
       <c r="A111" t="s">
         <v>107</v>
       </c>
@@ -1939,7 +1938,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3">
       <c r="A112" t="s">
         <v>108</v>
       </c>
@@ -1947,7 +1946,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3">
       <c r="A113" t="s">
         <v>109</v>
       </c>
@@ -1955,7 +1954,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3">
       <c r="A114" t="s">
         <v>110</v>
       </c>
@@ -1963,7 +1962,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3">
       <c r="A115" t="s">
         <v>111</v>
       </c>
@@ -1971,7 +1970,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3">
       <c r="A116" t="s">
         <v>112</v>
       </c>
@@ -1979,7 +1978,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3">
       <c r="A117" t="s">
         <v>113</v>
       </c>
@@ -1987,7 +1986,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3">
       <c r="A118" t="s">
         <v>114</v>
       </c>
@@ -1995,7 +1994,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3">
       <c r="A119" t="s">
         <v>115</v>
       </c>
@@ -2003,7 +2002,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3">
       <c r="A120" t="s">
         <v>116</v>
       </c>
@@ -2011,7 +2010,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3">
       <c r="A121" t="s">
         <v>117</v>
       </c>
@@ -2019,7 +2018,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3">
       <c r="A122" t="s">
         <v>118</v>
       </c>
@@ -2027,7 +2026,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3">
       <c r="A123" t="s">
         <v>119</v>
       </c>
@@ -2035,7 +2034,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3">
       <c r="A124" t="s">
         <v>120</v>
       </c>
@@ -2043,7 +2042,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3">
       <c r="A125" t="s">
         <v>121</v>
       </c>
@@ -2051,7 +2050,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3">
       <c r="A126" t="s">
         <v>122</v>
       </c>
@@ -2059,7 +2058,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3">
       <c r="A127" t="s">
         <v>123</v>
       </c>
@@ -2067,7 +2066,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3">
       <c r="A128" t="s">
         <v>124</v>
       </c>
@@ -2075,7 +2074,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3">
       <c r="A129" t="s">
         <v>125</v>
       </c>
@@ -2083,7 +2082,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3">
       <c r="A130" t="s">
         <v>126</v>
       </c>
@@ -2091,7 +2090,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3">
       <c r="A131" t="s">
         <v>127</v>
       </c>
@@ -2099,7 +2098,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3">
       <c r="A132" t="s">
         <v>128</v>
       </c>
@@ -2110,7 +2109,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3">
       <c r="A133" t="s">
         <v>129</v>
       </c>
@@ -2118,7 +2117,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3">
       <c r="A134" t="s">
         <v>130</v>
       </c>
@@ -2126,7 +2125,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3">
       <c r="A135" t="s">
         <v>131</v>
       </c>
@@ -2134,7 +2133,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3">
       <c r="A136" t="s">
         <v>132</v>
       </c>
@@ -2142,7 +2141,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3">
       <c r="A137" t="s">
         <v>133</v>
       </c>
@@ -2150,7 +2149,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3">
       <c r="A138" t="s">
         <v>134</v>
       </c>
@@ -2158,7 +2157,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3">
       <c r="A139" t="s">
         <v>135</v>
       </c>
@@ -2166,7 +2165,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3">
       <c r="A140" t="s">
         <v>136</v>
       </c>
@@ -2174,7 +2173,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3">
       <c r="A141" t="s">
         <v>137</v>
       </c>
@@ -2182,7 +2181,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3">
       <c r="A142" t="s">
         <v>138</v>
       </c>
@@ -2190,7 +2189,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3">
       <c r="A143" t="s">
         <v>139</v>
       </c>
@@ -2198,7 +2197,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3">
       <c r="A144" t="s">
         <v>140</v>
       </c>
@@ -2206,7 +2205,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3">
       <c r="A145" t="s">
         <v>141</v>
       </c>
@@ -2214,7 +2213,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3">
       <c r="A146" t="s">
         <v>142</v>
       </c>
@@ -2222,7 +2221,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3">
       <c r="A147" t="s">
         <v>139</v>
       </c>
@@ -2230,7 +2229,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3">
       <c r="A148" t="s">
         <v>140</v>
       </c>
@@ -2238,7 +2237,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3">
       <c r="A149" t="s">
         <v>141</v>
       </c>
@@ -2246,7 +2245,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3">
       <c r="A150" t="s">
         <v>142</v>
       </c>
@@ -2254,7 +2253,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3">
       <c r="A151" t="s">
         <v>143</v>
       </c>
@@ -2262,7 +2261,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3">
       <c r="A152" t="s">
         <v>144</v>
       </c>
@@ -2270,7 +2269,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3">
       <c r="A153" t="s">
         <v>145</v>
       </c>
@@ -2278,7 +2277,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3">
       <c r="A154" t="s">
         <v>146</v>
       </c>
@@ -2286,7 +2285,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3">
       <c r="A155" t="s">
         <v>147</v>
       </c>
@@ -2294,7 +2293,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3">
       <c r="A156" t="s">
         <v>148</v>
       </c>
@@ -2302,7 +2301,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3">
       <c r="A157" t="s">
         <v>149</v>
       </c>
@@ -2310,7 +2309,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3">
       <c r="A158" t="s">
         <v>150</v>
       </c>
@@ -2318,7 +2317,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3">
       <c r="A159" t="s">
         <v>151</v>
       </c>
@@ -2326,7 +2325,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3">
       <c r="A160" t="s">
         <v>152</v>
       </c>
@@ -2334,7 +2333,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3">
       <c r="A161" t="s">
         <v>153</v>
       </c>
@@ -2342,7 +2341,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3">
       <c r="A162" t="s">
         <v>154</v>
       </c>
@@ -2350,7 +2349,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3">
       <c r="A163" t="s">
         <v>155</v>
       </c>
@@ -2358,7 +2357,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3">
       <c r="A164" t="s">
         <v>156</v>
       </c>
@@ -2366,7 +2365,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3">
       <c r="A165" t="s">
         <v>157</v>
       </c>
@@ -2374,7 +2373,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3">
       <c r="A166" t="s">
         <v>158</v>
       </c>
@@ -2382,7 +2381,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3">
       <c r="A167" t="s">
         <v>159</v>
       </c>
@@ -2390,7 +2389,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3">
       <c r="A168" t="s">
         <v>160</v>
       </c>
@@ -2398,7 +2397,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3">
       <c r="A169" t="s">
         <v>161</v>
       </c>
@@ -2406,7 +2405,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3">
       <c r="A170" t="s">
         <v>162</v>
       </c>
@@ -2414,7 +2413,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3">
       <c r="A171" t="s">
         <v>163</v>
       </c>
@@ -2422,7 +2421,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3">
       <c r="A172" t="s">
         <v>164</v>
       </c>
@@ -2430,7 +2429,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3">
       <c r="A173" t="s">
         <v>165</v>
       </c>
@@ -2438,7 +2437,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3">
       <c r="A174" t="s">
         <v>166</v>
       </c>
@@ -2446,7 +2445,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3">
       <c r="A175" t="s">
         <v>167</v>
       </c>
@@ -2454,7 +2453,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3">
       <c r="A176" t="s">
         <v>168</v>
       </c>
@@ -2462,7 +2461,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3">
       <c r="A177" t="s">
         <v>169</v>
       </c>
@@ -2470,7 +2469,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3">
       <c r="A178" t="s">
         <v>170</v>
       </c>
@@ -2478,7 +2477,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3">
       <c r="A179" t="s">
         <v>171</v>
       </c>
@@ -2486,7 +2485,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3">
       <c r="A180" t="s">
         <v>172</v>
       </c>
@@ -2494,7 +2493,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3">
       <c r="A181" t="s">
         <v>173</v>
       </c>
@@ -2502,7 +2501,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3">
       <c r="A182" t="s">
         <v>174</v>
       </c>
@@ -2510,7 +2509,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3">
       <c r="A183" t="s">
         <v>175</v>
       </c>
@@ -2518,7 +2517,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3">
       <c r="A184" t="s">
         <v>176</v>
       </c>
@@ -2526,7 +2525,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3">
       <c r="A185" t="s">
         <v>177</v>
       </c>
@@ -2534,7 +2533,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3">
       <c r="A186" t="s">
         <v>178</v>
       </c>
@@ -2542,7 +2541,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3">
       <c r="A187" t="s">
         <v>179</v>
       </c>
@@ -2550,7 +2549,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3">
       <c r="A188" t="s">
         <v>180</v>
       </c>
@@ -2558,7 +2557,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3">
       <c r="A189" t="s">
         <v>181</v>
       </c>
@@ -2566,7 +2565,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3">
       <c r="A190" t="s">
         <v>182</v>
       </c>
@@ -2574,7 +2573,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3">
       <c r="A191" t="s">
         <v>183</v>
       </c>
@@ -2582,7 +2581,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3">
       <c r="A192" t="s">
         <v>184</v>
       </c>
@@ -2590,7 +2589,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3">
       <c r="A193" t="s">
         <v>185</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3">
       <c r="A194" t="s">
         <v>186</v>
       </c>
@@ -2606,7 +2605,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3">
       <c r="A195" t="s">
         <v>187</v>
       </c>
@@ -2614,7 +2613,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3">
       <c r="A196" t="s">
         <v>188</v>
       </c>
@@ -2622,7 +2621,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3">
       <c r="A197" t="s">
         <v>189</v>
       </c>
@@ -2630,7 +2629,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3">
       <c r="A198" t="s">
         <v>190</v>
       </c>
@@ -2638,7 +2637,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3">
       <c r="A199" t="s">
         <v>191</v>
       </c>
@@ -2646,7 +2645,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3">
       <c r="A200" t="s">
         <v>192</v>
       </c>
@@ -2654,7 +2653,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3">
       <c r="A201" t="s">
         <v>193</v>
       </c>

</xml_diff>